<commit_message>
01.12.2020 MC SaleS Details
</commit_message>
<xml_diff>
--- a/2020/November/All Details/30.11.2020/MC Bank Statement November-2020.xlsx
+++ b/2020/November/All Details/30.11.2020/MC Bank Statement November-2020.xlsx
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="227">
   <si>
     <t>Date</t>
   </si>
@@ -3061,18 +3061,54 @@
     <xf numFmtId="0" fontId="39" fillId="35" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="41" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="41" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="41" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3083,42 +3119,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="41" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="41" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="41" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3212,7 +3212,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3224,7 +3224,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3247,14 +3247,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3291,7 +3291,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3303,7 +3303,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3326,14 +3326,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3365,7 +3365,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3377,7 +3377,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3400,14 +3400,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4974,8 +4974,8 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -5277,9 +5277,7 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="55"/>
-      <c r="H9" s="28" t="s">
-        <v>183</v>
-      </c>
+      <c r="H9" s="28"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -21873,94 +21871,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="311" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="319"/>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
-      <c r="F1" s="319"/>
-      <c r="G1" s="319"/>
-      <c r="H1" s="319"/>
-      <c r="I1" s="319"/>
-      <c r="J1" s="319"/>
-      <c r="K1" s="319"/>
-      <c r="L1" s="319"/>
-      <c r="M1" s="319"/>
-      <c r="N1" s="319"/>
-      <c r="O1" s="319"/>
-      <c r="P1" s="319"/>
-      <c r="Q1" s="319"/>
-      <c r="R1" s="319"/>
-      <c r="S1" s="319"/>
+      <c r="B1" s="311"/>
+      <c r="C1" s="311"/>
+      <c r="D1" s="311"/>
+      <c r="E1" s="311"/>
+      <c r="F1" s="311"/>
+      <c r="G1" s="311"/>
+      <c r="H1" s="311"/>
+      <c r="I1" s="311"/>
+      <c r="J1" s="311"/>
+      <c r="K1" s="311"/>
+      <c r="L1" s="311"/>
+      <c r="M1" s="311"/>
+      <c r="N1" s="311"/>
+      <c r="O1" s="311"/>
+      <c r="P1" s="311"/>
+      <c r="Q1" s="311"/>
+      <c r="R1" s="311"/>
+      <c r="S1" s="311"/>
     </row>
     <row r="2" spans="1:26" s="204" customFormat="1" ht="18">
-      <c r="A2" s="320" t="s">
+      <c r="A2" s="312" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="320"/>
-      <c r="C2" s="320"/>
-      <c r="D2" s="320"/>
-      <c r="E2" s="320"/>
-      <c r="F2" s="320"/>
-      <c r="G2" s="320"/>
-      <c r="H2" s="320"/>
-      <c r="I2" s="320"/>
-      <c r="J2" s="320"/>
-      <c r="K2" s="320"/>
-      <c r="L2" s="320"/>
-      <c r="M2" s="320"/>
-      <c r="N2" s="320"/>
-      <c r="O2" s="320"/>
-      <c r="P2" s="320"/>
-      <c r="Q2" s="320"/>
-      <c r="R2" s="320"/>
-      <c r="S2" s="320"/>
+      <c r="B2" s="312"/>
+      <c r="C2" s="312"/>
+      <c r="D2" s="312"/>
+      <c r="E2" s="312"/>
+      <c r="F2" s="312"/>
+      <c r="G2" s="312"/>
+      <c r="H2" s="312"/>
+      <c r="I2" s="312"/>
+      <c r="J2" s="312"/>
+      <c r="K2" s="312"/>
+      <c r="L2" s="312"/>
+      <c r="M2" s="312"/>
+      <c r="N2" s="312"/>
+      <c r="O2" s="312"/>
+      <c r="P2" s="312"/>
+      <c r="Q2" s="312"/>
+      <c r="R2" s="312"/>
+      <c r="S2" s="312"/>
     </row>
     <row r="3" spans="1:26" s="204" customFormat="1">
-      <c r="A3" s="321"/>
-      <c r="B3" s="321"/>
-      <c r="C3" s="321"/>
-      <c r="D3" s="321"/>
-      <c r="E3" s="321"/>
-      <c r="F3" s="321"/>
-      <c r="G3" s="321"/>
-      <c r="H3" s="321"/>
-      <c r="I3" s="321"/>
-      <c r="J3" s="321"/>
-      <c r="K3" s="321"/>
-      <c r="L3" s="321"/>
-      <c r="M3" s="321"/>
-      <c r="N3" s="321"/>
-      <c r="O3" s="321"/>
-      <c r="P3" s="321"/>
-      <c r="Q3" s="321"/>
-      <c r="R3" s="321"/>
-      <c r="S3" s="321"/>
+      <c r="A3" s="313"/>
+      <c r="B3" s="313"/>
+      <c r="C3" s="313"/>
+      <c r="D3" s="313"/>
+      <c r="E3" s="313"/>
+      <c r="F3" s="313"/>
+      <c r="G3" s="313"/>
+      <c r="H3" s="313"/>
+      <c r="I3" s="313"/>
+      <c r="J3" s="313"/>
+      <c r="K3" s="313"/>
+      <c r="L3" s="313"/>
+      <c r="M3" s="313"/>
+      <c r="N3" s="313"/>
+      <c r="O3" s="313"/>
+      <c r="P3" s="313"/>
+      <c r="Q3" s="313"/>
+      <c r="R3" s="313"/>
+      <c r="S3" s="313"/>
     </row>
     <row r="4" spans="1:26" s="205" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="322" t="s">
+      <c r="A4" s="314" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="323"/>
-      <c r="C4" s="323"/>
-      <c r="D4" s="323"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="323"/>
-      <c r="G4" s="323"/>
-      <c r="H4" s="323"/>
-      <c r="I4" s="323"/>
-      <c r="J4" s="323"/>
-      <c r="K4" s="323"/>
-      <c r="L4" s="323"/>
-      <c r="M4" s="323"/>
-      <c r="N4" s="323"/>
-      <c r="O4" s="323"/>
-      <c r="P4" s="323"/>
-      <c r="Q4" s="323"/>
-      <c r="R4" s="323"/>
-      <c r="S4" s="324"/>
+      <c r="B4" s="315"/>
+      <c r="C4" s="315"/>
+      <c r="D4" s="315"/>
+      <c r="E4" s="315"/>
+      <c r="F4" s="315"/>
+      <c r="G4" s="315"/>
+      <c r="H4" s="315"/>
+      <c r="I4" s="315"/>
+      <c r="J4" s="315"/>
+      <c r="K4" s="315"/>
+      <c r="L4" s="315"/>
+      <c r="M4" s="315"/>
+      <c r="N4" s="315"/>
+      <c r="O4" s="315"/>
+      <c r="P4" s="315"/>
+      <c r="Q4" s="315"/>
+      <c r="R4" s="315"/>
+      <c r="S4" s="316"/>
       <c r="U4" s="116"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
@@ -21969,58 +21967,58 @@
       <c r="Z4" s="29"/>
     </row>
     <row r="5" spans="1:26" s="207" customFormat="1">
-      <c r="A5" s="325" t="s">
+      <c r="A5" s="317" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="327" t="s">
+      <c r="B5" s="319" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="313" t="s">
+      <c r="C5" s="321" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="313" t="s">
+      <c r="D5" s="321" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="313" t="s">
+      <c r="E5" s="321" t="s">
         <v>120</v>
       </c>
-      <c r="F5" s="313" t="s">
+      <c r="F5" s="321" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="313" t="s">
+      <c r="G5" s="321" t="s">
         <v>122</v>
       </c>
-      <c r="H5" s="313" t="s">
+      <c r="H5" s="321" t="s">
         <v>123</v>
       </c>
-      <c r="I5" s="313" t="s">
+      <c r="I5" s="321" t="s">
         <v>164</v>
       </c>
-      <c r="J5" s="313" t="s">
+      <c r="J5" s="321" t="s">
         <v>124</v>
       </c>
-      <c r="K5" s="313" t="s">
+      <c r="K5" s="321" t="s">
         <v>125</v>
       </c>
-      <c r="L5" s="313" t="s">
+      <c r="L5" s="321" t="s">
         <v>126</v>
       </c>
-      <c r="M5" s="313" t="s">
+      <c r="M5" s="321" t="s">
         <v>127</v>
       </c>
-      <c r="N5" s="313" t="s">
+      <c r="N5" s="321" t="s">
         <v>128</v>
       </c>
-      <c r="O5" s="315" t="s">
+      <c r="O5" s="327" t="s">
         <v>129</v>
       </c>
-      <c r="P5" s="317" t="s">
+      <c r="P5" s="329" t="s">
         <v>130</v>
       </c>
-      <c r="Q5" s="311" t="s">
+      <c r="Q5" s="325" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="329" t="s">
+      <c r="R5" s="323" t="s">
         <v>131</v>
       </c>
       <c r="S5" s="206" t="s">
@@ -22033,24 +22031,24 @@
       <c r="Y5" s="209"/>
     </row>
     <row r="6" spans="1:26" s="207" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A6" s="326"/>
-      <c r="B6" s="328"/>
-      <c r="C6" s="314"/>
-      <c r="D6" s="314"/>
-      <c r="E6" s="314"/>
-      <c r="F6" s="314"/>
-      <c r="G6" s="314"/>
-      <c r="H6" s="314"/>
-      <c r="I6" s="314"/>
-      <c r="J6" s="314"/>
-      <c r="K6" s="314"/>
-      <c r="L6" s="314"/>
-      <c r="M6" s="314"/>
-      <c r="N6" s="314"/>
-      <c r="O6" s="316"/>
-      <c r="P6" s="318"/>
-      <c r="Q6" s="312"/>
-      <c r="R6" s="330"/>
+      <c r="A6" s="318"/>
+      <c r="B6" s="320"/>
+      <c r="C6" s="322"/>
+      <c r="D6" s="322"/>
+      <c r="E6" s="322"/>
+      <c r="F6" s="322"/>
+      <c r="G6" s="322"/>
+      <c r="H6" s="322"/>
+      <c r="I6" s="322"/>
+      <c r="J6" s="322"/>
+      <c r="K6" s="322"/>
+      <c r="L6" s="322"/>
+      <c r="M6" s="322"/>
+      <c r="N6" s="322"/>
+      <c r="O6" s="328"/>
+      <c r="P6" s="330"/>
+      <c r="Q6" s="326"/>
+      <c r="R6" s="324"/>
       <c r="S6" s="211" t="s">
         <v>132</v>
       </c>
@@ -25407,6 +25405,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -25423,12 +25427,6 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
09.12.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/November/All Details/30.11.2020/MC Bank Statement November-2020.xlsx
+++ b/2020/November/All Details/30.11.2020/MC Bank Statement November-2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Nov 2020" sheetId="7" r:id="rId1"/>
@@ -3061,6 +3061,30 @@
     <xf numFmtId="0" fontId="39" fillId="35" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3091,34 +3115,10 @@
     <xf numFmtId="1" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3212,7 +3212,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3224,7 +3224,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3247,14 +3247,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3291,7 +3291,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3303,7 +3303,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3326,14 +3326,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3365,7 +3365,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3377,7 +3377,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3400,14 +3400,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4974,7 +4974,7 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -10690,8 +10690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI246"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -21871,94 +21871,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="311" t="s">
+      <c r="A1" s="319" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="311"/>
-      <c r="C1" s="311"/>
-      <c r="D1" s="311"/>
-      <c r="E1" s="311"/>
-      <c r="F1" s="311"/>
-      <c r="G1" s="311"/>
-      <c r="H1" s="311"/>
-      <c r="I1" s="311"/>
-      <c r="J1" s="311"/>
-      <c r="K1" s="311"/>
-      <c r="L1" s="311"/>
-      <c r="M1" s="311"/>
-      <c r="N1" s="311"/>
-      <c r="O1" s="311"/>
-      <c r="P1" s="311"/>
-      <c r="Q1" s="311"/>
-      <c r="R1" s="311"/>
-      <c r="S1" s="311"/>
+      <c r="B1" s="319"/>
+      <c r="C1" s="319"/>
+      <c r="D1" s="319"/>
+      <c r="E1" s="319"/>
+      <c r="F1" s="319"/>
+      <c r="G1" s="319"/>
+      <c r="H1" s="319"/>
+      <c r="I1" s="319"/>
+      <c r="J1" s="319"/>
+      <c r="K1" s="319"/>
+      <c r="L1" s="319"/>
+      <c r="M1" s="319"/>
+      <c r="N1" s="319"/>
+      <c r="O1" s="319"/>
+      <c r="P1" s="319"/>
+      <c r="Q1" s="319"/>
+      <c r="R1" s="319"/>
+      <c r="S1" s="319"/>
     </row>
     <row r="2" spans="1:26" s="204" customFormat="1" ht="18">
-      <c r="A2" s="312" t="s">
+      <c r="A2" s="320" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="312"/>
-      <c r="C2" s="312"/>
-      <c r="D2" s="312"/>
-      <c r="E2" s="312"/>
-      <c r="F2" s="312"/>
-      <c r="G2" s="312"/>
-      <c r="H2" s="312"/>
-      <c r="I2" s="312"/>
-      <c r="J2" s="312"/>
-      <c r="K2" s="312"/>
-      <c r="L2" s="312"/>
-      <c r="M2" s="312"/>
-      <c r="N2" s="312"/>
-      <c r="O2" s="312"/>
-      <c r="P2" s="312"/>
-      <c r="Q2" s="312"/>
-      <c r="R2" s="312"/>
-      <c r="S2" s="312"/>
+      <c r="B2" s="320"/>
+      <c r="C2" s="320"/>
+      <c r="D2" s="320"/>
+      <c r="E2" s="320"/>
+      <c r="F2" s="320"/>
+      <c r="G2" s="320"/>
+      <c r="H2" s="320"/>
+      <c r="I2" s="320"/>
+      <c r="J2" s="320"/>
+      <c r="K2" s="320"/>
+      <c r="L2" s="320"/>
+      <c r="M2" s="320"/>
+      <c r="N2" s="320"/>
+      <c r="O2" s="320"/>
+      <c r="P2" s="320"/>
+      <c r="Q2" s="320"/>
+      <c r="R2" s="320"/>
+      <c r="S2" s="320"/>
     </row>
     <row r="3" spans="1:26" s="204" customFormat="1">
-      <c r="A3" s="313"/>
-      <c r="B3" s="313"/>
-      <c r="C3" s="313"/>
-      <c r="D3" s="313"/>
-      <c r="E3" s="313"/>
-      <c r="F3" s="313"/>
-      <c r="G3" s="313"/>
-      <c r="H3" s="313"/>
-      <c r="I3" s="313"/>
-      <c r="J3" s="313"/>
-      <c r="K3" s="313"/>
-      <c r="L3" s="313"/>
-      <c r="M3" s="313"/>
-      <c r="N3" s="313"/>
-      <c r="O3" s="313"/>
-      <c r="P3" s="313"/>
-      <c r="Q3" s="313"/>
-      <c r="R3" s="313"/>
-      <c r="S3" s="313"/>
+      <c r="A3" s="321"/>
+      <c r="B3" s="321"/>
+      <c r="C3" s="321"/>
+      <c r="D3" s="321"/>
+      <c r="E3" s="321"/>
+      <c r="F3" s="321"/>
+      <c r="G3" s="321"/>
+      <c r="H3" s="321"/>
+      <c r="I3" s="321"/>
+      <c r="J3" s="321"/>
+      <c r="K3" s="321"/>
+      <c r="L3" s="321"/>
+      <c r="M3" s="321"/>
+      <c r="N3" s="321"/>
+      <c r="O3" s="321"/>
+      <c r="P3" s="321"/>
+      <c r="Q3" s="321"/>
+      <c r="R3" s="321"/>
+      <c r="S3" s="321"/>
     </row>
     <row r="4" spans="1:26" s="205" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="314" t="s">
+      <c r="A4" s="322" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="315"/>
-      <c r="C4" s="315"/>
-      <c r="D4" s="315"/>
-      <c r="E4" s="315"/>
-      <c r="F4" s="315"/>
-      <c r="G4" s="315"/>
-      <c r="H4" s="315"/>
-      <c r="I4" s="315"/>
-      <c r="J4" s="315"/>
-      <c r="K4" s="315"/>
-      <c r="L4" s="315"/>
-      <c r="M4" s="315"/>
-      <c r="N4" s="315"/>
-      <c r="O4" s="315"/>
-      <c r="P4" s="315"/>
-      <c r="Q4" s="315"/>
-      <c r="R4" s="315"/>
-      <c r="S4" s="316"/>
+      <c r="B4" s="323"/>
+      <c r="C4" s="323"/>
+      <c r="D4" s="323"/>
+      <c r="E4" s="323"/>
+      <c r="F4" s="323"/>
+      <c r="G4" s="323"/>
+      <c r="H4" s="323"/>
+      <c r="I4" s="323"/>
+      <c r="J4" s="323"/>
+      <c r="K4" s="323"/>
+      <c r="L4" s="323"/>
+      <c r="M4" s="323"/>
+      <c r="N4" s="323"/>
+      <c r="O4" s="323"/>
+      <c r="P4" s="323"/>
+      <c r="Q4" s="323"/>
+      <c r="R4" s="323"/>
+      <c r="S4" s="324"/>
       <c r="U4" s="116"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
@@ -21967,58 +21967,58 @@
       <c r="Z4" s="29"/>
     </row>
     <row r="5" spans="1:26" s="207" customFormat="1">
-      <c r="A5" s="317" t="s">
+      <c r="A5" s="325" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="319" t="s">
+      <c r="B5" s="327" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="321" t="s">
+      <c r="C5" s="313" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="321" t="s">
+      <c r="D5" s="313" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="321" t="s">
+      <c r="E5" s="313" t="s">
         <v>120</v>
       </c>
-      <c r="F5" s="321" t="s">
+      <c r="F5" s="313" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="321" t="s">
+      <c r="G5" s="313" t="s">
         <v>122</v>
       </c>
-      <c r="H5" s="321" t="s">
+      <c r="H5" s="313" t="s">
         <v>123</v>
       </c>
-      <c r="I5" s="321" t="s">
+      <c r="I5" s="313" t="s">
         <v>164</v>
       </c>
-      <c r="J5" s="321" t="s">
+      <c r="J5" s="313" t="s">
         <v>124</v>
       </c>
-      <c r="K5" s="321" t="s">
+      <c r="K5" s="313" t="s">
         <v>125</v>
       </c>
-      <c r="L5" s="321" t="s">
+      <c r="L5" s="313" t="s">
         <v>126</v>
       </c>
-      <c r="M5" s="321" t="s">
+      <c r="M5" s="313" t="s">
         <v>127</v>
       </c>
-      <c r="N5" s="321" t="s">
+      <c r="N5" s="313" t="s">
         <v>128</v>
       </c>
-      <c r="O5" s="327" t="s">
+      <c r="O5" s="315" t="s">
         <v>129</v>
       </c>
-      <c r="P5" s="329" t="s">
+      <c r="P5" s="317" t="s">
         <v>130</v>
       </c>
-      <c r="Q5" s="325" t="s">
+      <c r="Q5" s="311" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="323" t="s">
+      <c r="R5" s="329" t="s">
         <v>131</v>
       </c>
       <c r="S5" s="206" t="s">
@@ -22031,24 +22031,24 @@
       <c r="Y5" s="209"/>
     </row>
     <row r="6" spans="1:26" s="207" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A6" s="318"/>
-      <c r="B6" s="320"/>
-      <c r="C6" s="322"/>
-      <c r="D6" s="322"/>
-      <c r="E6" s="322"/>
-      <c r="F6" s="322"/>
-      <c r="G6" s="322"/>
-      <c r="H6" s="322"/>
-      <c r="I6" s="322"/>
-      <c r="J6" s="322"/>
-      <c r="K6" s="322"/>
-      <c r="L6" s="322"/>
-      <c r="M6" s="322"/>
-      <c r="N6" s="322"/>
-      <c r="O6" s="328"/>
-      <c r="P6" s="330"/>
-      <c r="Q6" s="326"/>
-      <c r="R6" s="324"/>
+      <c r="A6" s="326"/>
+      <c r="B6" s="328"/>
+      <c r="C6" s="314"/>
+      <c r="D6" s="314"/>
+      <c r="E6" s="314"/>
+      <c r="F6" s="314"/>
+      <c r="G6" s="314"/>
+      <c r="H6" s="314"/>
+      <c r="I6" s="314"/>
+      <c r="J6" s="314"/>
+      <c r="K6" s="314"/>
+      <c r="L6" s="314"/>
+      <c r="M6" s="314"/>
+      <c r="N6" s="314"/>
+      <c r="O6" s="316"/>
+      <c r="P6" s="318"/>
+      <c r="Q6" s="312"/>
+      <c r="R6" s="330"/>
       <c r="S6" s="211" t="s">
         <v>132</v>
       </c>
@@ -25405,12 +25405,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -25427,6 +25421,12 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>